<commit_message>
Refactor and add support for arbitrary CSV delimiters
Also:

* Switch from ' to " for strings literals.
* Replace the Makefile with a shell script.
* Update Readme.
</commit_message>
<xml_diff>
--- a/example/example1.xlsx
+++ b/example/example1.xlsx
@@ -47,13 +47,13 @@
     <t xml:space="preserve">six seven</t>
   </si>
   <si>
-    <t xml:space="preserve">ddd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">eee</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fff ggg</t>
+    <t xml:space="preserve">2dd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EEE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fff ggg_?h’i</t>
   </si>
   <si>
     <t xml:space="preserve">eight</t>
@@ -86,6 +86,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -107,6 +108,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -158,8 +160,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -190,38 +196,38 @@
       <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="1" t="n">
         <v>111</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -244,41 +250,41 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J4" activeCellId="0" sqref="J4"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>